<commit_message>
All the code tested sucessfully
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
+++ b/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvkrishnarao/Desktop/RA/Intelligibility_Software_Module/Audio_Files/Person_1/Intelligibility_Score/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F663F60E-8C32-B146-82C3-C308A1B392F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="1700" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Score_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -58,59 +52,59 @@
     <t>Test8</t>
   </si>
   <si>
+    <t>P1_W2_S1</t>
+  </si>
+  <si>
+    <t>P1_W2_S4</t>
+  </si>
+  <si>
+    <t>P1_W2_S2</t>
+  </si>
+  <si>
+    <t>P1_W2_S3</t>
+  </si>
+  <si>
+    <t>P1_W1_S1</t>
+  </si>
+  <si>
     <t>P1_W1_S4</t>
   </si>
   <si>
+    <t>P1_W1_S2</t>
+  </si>
+  <si>
     <t>P1_W1_S3</t>
   </si>
   <si>
-    <t>P1_W1_S2</t>
-  </si>
-  <si>
-    <t>P1_W1_S1</t>
-  </si>
-  <si>
-    <t>P1_W2_S4</t>
-  </si>
-  <si>
-    <t>P1_W2_S3</t>
-  </si>
-  <si>
-    <t>P1_W2_S2</t>
-  </si>
-  <si>
-    <t>P1_W2_S1</t>
+    <t>I think I'm getting better.</t>
+  </si>
+  <si>
+    <t>he is capable and willing to make decisions.</t>
+  </si>
+  <si>
+    <t>You want him to do well</t>
+  </si>
+  <si>
+    <t>Big muscles are not necessarily strong ones</t>
+  </si>
+  <si>
+    <t>We picked grapes for wine</t>
   </si>
   <si>
     <t>Enjoy the fair weather while in the tropics.</t>
   </si>
   <si>
+    <t>The ballet is about to begin.</t>
+  </si>
+  <si>
     <t>You're used to being on the field.</t>
-  </si>
-  <si>
-    <t>The ballet is about to begin.</t>
-  </si>
-  <si>
-    <t>We picked grapes for wine</t>
-  </si>
-  <si>
-    <t>he is capable and willing to make decisions.</t>
-  </si>
-  <si>
-    <t>Big muscles are not necessarily strong ones</t>
-  </si>
-  <si>
-    <t>You want him to do well</t>
-  </si>
-  <si>
-    <t>I think I'm getting better.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +167,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -227,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,27 +245,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,24 +279,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,23 +454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -548,10 +489,10 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>8.1632653061224483E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -565,10 +506,10 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>0.15384615384615391</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1224489795918367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -582,10 +523,10 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <v>0.1764705882352941</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1428571428571428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -599,10 +540,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>0.1333333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -616,10 +557,10 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <v>0.1224489795918367</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -633,10 +574,10 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.08163265306122448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -650,10 +591,10 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.14285714285714279</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.1764705882352941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -667,7 +608,7 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>0.125</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushed a few changes
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
+++ b/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
@@ -52,52 +52,52 @@
     <t>Test8</t>
   </si>
   <si>
+    <t>P1_W1_S4</t>
+  </si>
+  <si>
+    <t>P1_W1_S1</t>
+  </si>
+  <si>
+    <t>P1_W1_S2</t>
+  </si>
+  <si>
+    <t>P1_W1_S3</t>
+  </si>
+  <si>
+    <t>P1_W2_S4</t>
+  </si>
+  <si>
     <t>P1_W2_S1</t>
   </si>
   <si>
-    <t>P1_W2_S4</t>
-  </si>
-  <si>
     <t>P1_W2_S2</t>
   </si>
   <si>
     <t>P1_W2_S3</t>
   </si>
   <si>
-    <t>P1_W1_S1</t>
-  </si>
-  <si>
-    <t>P1_W1_S4</t>
-  </si>
-  <si>
-    <t>P1_W1_S2</t>
-  </si>
-  <si>
-    <t>P1_W1_S3</t>
+    <t>Enjoy the fair weather while in the tropics.</t>
+  </si>
+  <si>
+    <t>We picked grapes for wine</t>
+  </si>
+  <si>
+    <t>The ballet is about to begin.</t>
+  </si>
+  <si>
+    <t>You're used to being on the field.</t>
+  </si>
+  <si>
+    <t>he is capable and willing to make decisions.</t>
   </si>
   <si>
     <t>I think I'm getting better.</t>
   </si>
   <si>
-    <t>he is capable and willing to make decisions.</t>
-  </si>
-  <si>
     <t>You want him to do well</t>
   </si>
   <si>
     <t>Big muscles are not necessarily strong ones</t>
-  </si>
-  <si>
-    <t>We picked grapes for wine</t>
-  </si>
-  <si>
-    <t>Enjoy the fair weather while in the tropics.</t>
-  </si>
-  <si>
-    <t>The ballet is about to begin.</t>
-  </si>
-  <si>
-    <t>You're used to being on the field.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>0.125</v>
+        <v>0.08163265306122448</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -506,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>0.1224489795918367</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -523,7 +523,7 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <v>0.1428571428571428</v>
+        <v>0.1764705882352941</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -540,7 +540,7 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>0.125</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -557,7 +557,7 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <v>0.1333333333333333</v>
+        <v>0.1224489795918367</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -574,7 +574,7 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>0.08163265306122448</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -591,7 +591,7 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.1764705882352941</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -608,7 +608,7 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>0.1538461538461539</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried fixing the IndeXOutOfBound Error
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
+++ b/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
@@ -1,110 +1,116 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvkrishnarao/Desktop/RA/Intelligibility_Software_Module/Audio_Files/Person_1/Intelligibility_Score/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE215B85-37D0-F740-B8A5-13EAC4EF0D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Score_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
+    <t>SENTENCES</t>
+  </si>
+  <si>
     <t>INPUT_SENTENCE</t>
   </si>
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>SENTENCES</t>
-  </si>
-  <si>
     <t>INTELLIGIBILITY_SCORE</t>
   </si>
   <si>
+    <t>I think I'm getting better.</t>
+  </si>
+  <si>
+    <t>You want him to do well</t>
+  </si>
+  <si>
+    <t>Big muscles are not necessarily strong ones</t>
+  </si>
+  <si>
+    <t>he is capable and willing to make decisions.</t>
+  </si>
+  <si>
+    <t>We picked grapes for wine</t>
+  </si>
+  <si>
+    <t>The ballet is about to begin.</t>
+  </si>
+  <si>
+    <t>You're used to being on the field.</t>
+  </si>
+  <si>
+    <t>Enjoy the fair weather while in the tropics.</t>
+  </si>
+  <si>
     <t>Test1</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>Test6</t>
-  </si>
-  <si>
-    <t>Test7</t>
-  </si>
-  <si>
-    <t>Test8</t>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>P1_W2_S1</t>
+  </si>
+  <si>
+    <t>P1_W2_S2</t>
+  </si>
+  <si>
+    <t>P1_W2_S3</t>
+  </si>
+  <si>
+    <t>P1_W2_S4</t>
+  </si>
+  <si>
+    <t>P1_W1_S1</t>
+  </si>
+  <si>
+    <t>P1_W1_S2</t>
+  </si>
+  <si>
+    <t>P1_W1_S3</t>
   </si>
   <si>
     <t>P1_W1_S4</t>
-  </si>
-  <si>
-    <t>P1_W1_S1</t>
-  </si>
-  <si>
-    <t>P1_W1_S2</t>
-  </si>
-  <si>
-    <t>P1_W1_S3</t>
-  </si>
-  <si>
-    <t>P1_W2_S4</t>
-  </si>
-  <si>
-    <t>P1_W2_S1</t>
-  </si>
-  <si>
-    <t>P1_W2_S2</t>
-  </si>
-  <si>
-    <t>P1_W2_S3</t>
-  </si>
-  <si>
-    <t>Enjoy the fair weather while in the tropics.</t>
-  </si>
-  <si>
-    <t>We picked grapes for wine</t>
-  </si>
-  <si>
-    <t>The ballet is about to begin.</t>
-  </si>
-  <si>
-    <t>You're used to being on the field.</t>
-  </si>
-  <si>
-    <t>he is capable and willing to make decisions.</t>
-  </si>
-  <si>
-    <t>I think I'm getting better.</t>
-  </si>
-  <si>
-    <t>You want him to do well</t>
-  </si>
-  <si>
-    <t>Big muscles are not necessarily strong ones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +173,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +259,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +311,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +504,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -489,10 +548,10 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>0.08163265306122448</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -506,10 +565,10 @@
         <v>21</v>
       </c>
       <c r="E3">
-        <v>0.1333333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.14285714285714279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -523,10 +582,10 @@
         <v>22</v>
       </c>
       <c r="E4">
-        <v>0.1764705882352941</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -540,10 +599,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>0.1538461538461539</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.1224489795918367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -557,10 +616,10 @@
         <v>24</v>
       </c>
       <c r="E6">
-        <v>0.1224489795918367</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -574,10 +633,10 @@
         <v>25</v>
       </c>
       <c r="E7">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.1764705882352941</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -591,10 +650,10 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.1428571428571428</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.15384615384615391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -608,7 +667,7 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>0.125</v>
+        <v>8.1632653061224483E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some of the performance issues
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
+++ b/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cvkrishnarao/Desktop/RA/Intelligibility_Software_Module/Audio_Files/Person_1/Intelligibility_Score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D71038-3D49-9F4B-B591-6ECE479C4B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A62AE3-B732-574A-8FBD-DFAEFF2AFD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,52 +43,67 @@
     <t>Calculated_Intelligibility</t>
   </si>
   <si>
+    <t>he is capable and willing to make decisions.</t>
+  </si>
+  <si>
+    <t>Big muscles are not necessarily strong ones</t>
+  </si>
+  <si>
+    <t>I think I'm getting better.</t>
+  </si>
+  <si>
+    <t>You want him to do well</t>
+  </si>
+  <si>
+    <t>Enjoy the fair weather while in the tropics.</t>
+  </si>
+  <si>
     <t>You're used to being on the field.</t>
   </si>
   <si>
     <t>We picked grapes for wine</t>
   </si>
   <si>
-    <t>Enjoy the fair weather while in the tropics.</t>
-  </si>
-  <si>
     <t>The ballet is about to begin.</t>
   </si>
   <si>
-    <t>Big muscles are not necessarily strong ones</t>
-  </si>
-  <si>
-    <t>I think I'm getting better.</t>
-  </si>
-  <si>
-    <t>he is capable and willing to make decisions.</t>
-  </si>
-  <si>
-    <t>You want him to do well</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test7</t>
-  </si>
-  <si>
-    <t>test8</t>
+    <t>you want him to do well</t>
+  </si>
+  <si>
+    <t>he is capable and willing to decide</t>
+  </si>
+  <si>
+    <t>big muscles are not neccesarily strong</t>
+  </si>
+  <si>
+    <t>i think i'm getting better</t>
+  </si>
+  <si>
+    <t>the ballet is about to begin</t>
+  </si>
+  <si>
+    <t>enjoy the fair weather while in the tropics</t>
+  </si>
+  <si>
+    <t>your used to being on the feel</t>
+  </si>
+  <si>
+    <t>we picked grapes for wine</t>
+  </si>
+  <si>
+    <t>P1_W2_S4</t>
+  </si>
+  <si>
+    <t>P1_W2_S3</t>
+  </si>
+  <si>
+    <t>P1_W2_S1</t>
+  </si>
+  <si>
+    <t>P1_W2_S2</t>
+  </si>
+  <si>
+    <t>P1_W1_S4</t>
   </si>
   <si>
     <t>P1_W1_S3</t>
@@ -97,22 +112,7 @@
     <t>P1_W1_S1</t>
   </si>
   <si>
-    <t>P1_W1_S4</t>
-  </si>
-  <si>
     <t>P1_W1_S2</t>
-  </si>
-  <si>
-    <t>P1_W2_S3</t>
-  </si>
-  <si>
-    <t>P1_W2_S1</t>
-  </si>
-  <si>
-    <t>P1_W2_S4</t>
-  </si>
-  <si>
-    <t>P1_W2_S2</t>
   </si>
 </sst>
 </file>
@@ -517,14 +517,14 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -569,13 +569,13 @@
         <v>23</v>
       </c>
       <c r="E2">
-        <v>0.15384615384615391</v>
+        <v>0.29850746268656708</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -595,13 +595,13 @@
         <v>24</v>
       </c>
       <c r="E3">
-        <v>0.1333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -621,13 +621,13 @@
         <v>25</v>
       </c>
       <c r="E4">
-        <v>8.1632653061224483E-2</v>
+        <v>0.2461538461538462</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -647,7 +647,7 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>0.1764705882352941</v>
+        <v>0.36734693877551022</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -673,13 +673,13 @@
         <v>27</v>
       </c>
       <c r="E6">
-        <v>0.125</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -699,13 +699,13 @@
         <v>28</v>
       </c>
       <c r="E7">
-        <v>0.125</v>
+        <v>0.36363636363636359</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -725,13 +725,13 @@
         <v>29</v>
       </c>
       <c r="E8">
-        <v>0.1224489795918367</v>
+        <v>0.32727272727272733</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>30</v>
       </c>
       <c r="E9">
-        <v>0.14285714285714279</v>
+        <v>0.37037037037037029</v>
       </c>
       <c r="F9">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed the scoring system
</commit_message>
<xml_diff>
--- a/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
+++ b/Audio_Files/Person_1/Intelligibility_Score/Intelligibility_Score.xlsx
@@ -37,76 +37,76 @@
     <t>Calculated_Intelligibility</t>
   </si>
   <si>
+    <t>Enjoy the fair weather while in the tropics.</t>
+  </si>
+  <si>
+    <t>You're used to being on the field.</t>
+  </si>
+  <si>
+    <t>We picked grapes for wine</t>
+  </si>
+  <si>
     <t>The ballet is about to begin.</t>
   </si>
   <si>
-    <t>You're used to being on the field.</t>
-  </si>
-  <si>
-    <t>We picked grapes for wine</t>
-  </si>
-  <si>
-    <t>Enjoy the fair weather while in the tropics.</t>
+    <t>he is capable and willing to make decisions.</t>
+  </si>
+  <si>
+    <t>Big muscles are not necessarily strong ones</t>
+  </si>
+  <si>
+    <t>I think I'm getting better.</t>
   </si>
   <si>
     <t>You want him to do well</t>
   </si>
   <si>
-    <t>Big muscles are not necessarily strong ones</t>
-  </si>
-  <si>
-    <t>I think I'm getting better.</t>
-  </si>
-  <si>
-    <t>he is capable and willing to make decisions.</t>
-  </si>
-  <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>w2</t>
-  </si>
-  <si>
-    <t>e3</t>
-  </si>
-  <si>
-    <t>r4</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>y6</t>
-  </si>
-  <si>
-    <t>u7</t>
-  </si>
-  <si>
-    <t>i8</t>
+    <t>jewpofjoiwjFOJWROIFJWERFJOP[WKJEFPJKWF</t>
+  </si>
+  <si>
+    <t>PRKF[PJrwpvjwprjvp</t>
+  </si>
+  <si>
+    <t>khiuh wfhouhf ojhfojq oejfojq oijfojw oijwefojw jwoejfoi oijowj feohweoh</t>
+  </si>
+  <si>
+    <t>uhfowhoufh fweoij wefjowj ewfjojo efoijwo oijewoj efwjwo</t>
+  </si>
+  <si>
+    <t>owijefohj ohfweoh ewohfo efhweo fhjowhj fowejofj fjowej fewojo</t>
+  </si>
+  <si>
+    <t>whfi wefoh owjowj ojwfo fwjoj oefjoqj wfoijwo oewjoewj fjwojo wfjwojf ofewijfo</t>
+  </si>
+  <si>
+    <t>fnk hfow wrfh weojfo fwojo wroijfho ojwro fojoiwr ojwof jwfoi wjojo</t>
+  </si>
+  <si>
+    <t>ncaj ednfow woejfo jfowe weijfo pfjwoi foijwoi ewpijpo wpjfp ieoaij eijfp</t>
+  </si>
+  <si>
+    <t>P1_W1_S4</t>
+  </si>
+  <si>
+    <t>P1_W1_S3</t>
+  </si>
+  <si>
+    <t>P1_W1_S1</t>
   </si>
   <si>
     <t>P1_W1_S2</t>
   </si>
   <si>
-    <t>P1_W1_S3</t>
-  </si>
-  <si>
-    <t>P1_W1_S1</t>
-  </si>
-  <si>
-    <t>P1_W1_S4</t>
+    <t>P1_W2_S4</t>
+  </si>
+  <si>
+    <t>P1_W2_S3</t>
+  </si>
+  <si>
+    <t>P1_W2_S1</t>
   </si>
   <si>
     <t>P1_W2_S2</t>
-  </si>
-  <si>
-    <t>P1_W2_S3</t>
-  </si>
-  <si>
-    <t>P1_W2_S1</t>
-  </si>
-  <si>
-    <t>P1_W2_S4</t>
   </si>
 </sst>
 </file>
@@ -507,13 +507,13 @@
         <v>23</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.2439024390243902</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -533,7 +533,7 @@
         <v>24</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -559,13 +559,13 @@
         <v>25</v>
       </c>
       <c r="E4">
-        <v>0.07407407407407407</v>
+        <v>0.2061855670103093</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -585,13 +585,13 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>0.04347826086956522</v>
+        <v>0.1882352941176471</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -611,13 +611,13 @@
         <v>27</v>
       </c>
       <c r="E6">
-        <v>0.08</v>
+        <v>0.169811320754717</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -637,13 +637,13 @@
         <v>28</v>
       </c>
       <c r="E7">
-        <v>0.04444444444444445</v>
+        <v>0.115702479338843</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -663,13 +663,13 @@
         <v>29</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.148936170212766</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -689,13 +689,13 @@
         <v>30</v>
       </c>
       <c r="E9">
-        <v>0.04347826086956522</v>
+        <v>0.1875</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H9">
         <v>0</v>

</xml_diff>